<commit_message>
adicionado nova placa e organizacao
</commit_message>
<xml_diff>
--- a/Organizacao/Memorial de Calculo.xlsx
+++ b/Organizacao/Memorial de Calculo.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victor_roncalli\Documents\Concremat\Zinho\ConcRobo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victor_roncalli\Desktop\Projeto Zinho\DEVELOP\Organizacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Relação de Grandezas" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Codigo das Funcoes" sheetId="4" r:id="rId4"/>
     <sheet name="Bateria" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -264,18 +264,12 @@
     <t>accel.y</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>temperature</t>
   </si>
   <si>
     <t>pressure</t>
   </si>
   <si>
-    <t>battery</t>
-  </si>
-  <si>
     <t>light -</t>
   </si>
   <si>
@@ -385,14 +379,20 @@
   </si>
   <si>
     <t>Dist Max (m)</t>
+  </si>
+  <si>
+    <t>batCurrent</t>
+  </si>
+  <si>
+    <t>batTensao</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -589,21 +589,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -614,6 +602,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -634,9 +625,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2205,8 +2205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,20 +2234,20 @@
       <c r="E2" s="5"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="L2" s="37" t="s">
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="L2" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
     </row>
     <row r="3" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
@@ -2256,26 +2256,26 @@
       <c r="E3" s="5"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="L3" s="37" t="s">
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+      <c r="L3" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
     </row>
     <row r="4" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="37"/>
       <c r="F4" s="17" t="s">
         <v>63</v>
       </c>
@@ -2289,22 +2289,22 @@
       <c r="J4" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="33"/>
-      <c r="N4" s="36" t="s">
+      <c r="M4" s="46"/>
+      <c r="N4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36" t="s">
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="R4" s="36"/>
+      <c r="R4" s="34"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="38" t="s">
         <v>52</v>
       </c>
       <c r="D5" s="12" t="s">
@@ -2347,7 +2347,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="39"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="12" t="s">
         <v>53</v>
       </c>
@@ -2389,7 +2389,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="39"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="12" t="s">
         <v>27</v>
       </c>
@@ -2430,7 +2430,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="39"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="12" t="s">
         <v>54</v>
       </c>
@@ -2471,7 +2471,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="39"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="12" t="s">
         <v>33</v>
       </c>
@@ -2512,7 +2512,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="39"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="12" t="s">
         <v>55</v>
       </c>
@@ -2553,7 +2553,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="39"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="12" t="s">
         <v>56</v>
       </c>
@@ -2594,7 +2594,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="39"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="12" t="s">
         <v>57</v>
       </c>
@@ -2635,7 +2635,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C13" s="39"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="12" t="s">
         <v>24</v>
       </c>
@@ -2691,7 +2691,7 @@
       <c r="R14" s="6"/>
     </row>
     <row r="15" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="39" t="s">
         <v>74</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -2720,10 +2720,10 @@
         <f t="shared" ref="N15:N27" si="2">I15</f>
         <v>0x10</v>
       </c>
-      <c r="O15" s="29" t="s">
+      <c r="O15" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="P15" s="29"/>
+      <c r="P15" s="36"/>
       <c r="Q15" s="6" t="s">
         <v>66</v>
       </c>
@@ -2732,7 +2732,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="40"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="12" t="s">
         <v>77</v>
       </c>
@@ -2760,10 +2760,10 @@
         <f t="shared" si="2"/>
         <v>0x11</v>
       </c>
-      <c r="O16" s="29" t="s">
+      <c r="O16" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="P16" s="29"/>
+      <c r="P16" s="36"/>
       <c r="Q16" s="6" t="s">
         <v>66</v>
       </c>
@@ -2772,7 +2772,7 @@
       </c>
     </row>
     <row r="17" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C17" s="40"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="12" t="s">
         <v>75</v>
       </c>
@@ -2799,10 +2799,10 @@
         <f t="shared" si="2"/>
         <v>0x12</v>
       </c>
-      <c r="O17" s="29" t="s">
+      <c r="O17" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="P17" s="29"/>
+      <c r="P17" s="36"/>
       <c r="Q17" s="6" t="s">
         <v>66</v>
       </c>
@@ -2811,7 +2811,7 @@
       </c>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C18" s="40"/>
+      <c r="C18" s="39"/>
       <c r="D18" s="12"/>
       <c r="F18" s="6"/>
       <c r="H18" s="6"/>
@@ -2827,9 +2827,9 @@
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C19" s="40"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" s="6">
         <v>19</v>
@@ -2854,10 +2854,10 @@
         <f t="shared" ref="N19:N21" si="3">I19</f>
         <v>0x13</v>
       </c>
-      <c r="O19" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="P19" s="29"/>
+      <c r="O19" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="P19" s="36"/>
       <c r="Q19" s="6" t="s">
         <v>66</v>
       </c>
@@ -2866,9 +2866,9 @@
       </c>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C20" s="40"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" s="6">
         <v>20</v>
@@ -2893,10 +2893,10 @@
         <f t="shared" si="3"/>
         <v>0x14</v>
       </c>
-      <c r="O20" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="P20" s="29"/>
+      <c r="O20" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="P20" s="36"/>
       <c r="Q20" s="6" t="s">
         <v>66</v>
       </c>
@@ -2905,9 +2905,9 @@
       </c>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C21" s="40"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="12" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="F21" s="6">
         <v>21</v>
@@ -2932,10 +2932,10 @@
         <f t="shared" si="3"/>
         <v>0x15</v>
       </c>
-      <c r="O21" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="P21" s="29"/>
+      <c r="O21" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="P21" s="36"/>
       <c r="Q21" s="6" t="s">
         <v>66</v>
       </c>
@@ -2944,7 +2944,7 @@
       </c>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C22" s="40"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="12"/>
       <c r="F22" s="6"/>
       <c r="H22" s="6"/>
@@ -2959,9 +2959,9 @@
       <c r="R22" s="6"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C23" s="40"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F23" s="6">
         <v>22</v>
@@ -2983,12 +2983,12 @@
         <v>67</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="O23" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="P23" s="29"/>
+        <v>85</v>
+      </c>
+      <c r="O23" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="P23" s="36"/>
       <c r="Q23" s="6" t="s">
         <v>66</v>
       </c>
@@ -2997,9 +2997,9 @@
       </c>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C24" s="40"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F24" s="6">
         <v>23</v>
@@ -3021,12 +3021,12 @@
         <v>67</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="O24" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="P24" s="29"/>
+        <v>85</v>
+      </c>
+      <c r="O24" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="P24" s="36"/>
       <c r="Q24" s="6" t="s">
         <v>66</v>
       </c>
@@ -3035,9 +3035,9 @@
       </c>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="40"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F25" s="6">
         <v>24</v>
@@ -3046,7 +3046,7 @@
         <v>67</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>66</v>
@@ -3061,10 +3061,10 @@
         <f t="shared" ref="N25" si="4">I25</f>
         <v>0x18</v>
       </c>
-      <c r="O25" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="P25" s="29"/>
+      <c r="O25" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="P25" s="36"/>
       <c r="Q25" s="6" t="s">
         <v>66</v>
       </c>
@@ -3073,7 +3073,7 @@
       </c>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C26" s="40"/>
+      <c r="C26" s="39"/>
       <c r="D26" s="12"/>
       <c r="F26" s="6"/>
       <c r="H26" s="6"/>
@@ -3088,9 +3088,9 @@
       <c r="R26" s="6"/>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C27" s="40"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="12" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="F27" s="6">
         <v>24</v>
@@ -3099,7 +3099,7 @@
         <v>67</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>66</v>
@@ -3114,10 +3114,10 @@
         <f t="shared" si="2"/>
         <v>0x19</v>
       </c>
-      <c r="O27" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="P27" s="29"/>
+      <c r="O27" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="P27" s="36"/>
       <c r="Q27" s="6" t="s">
         <v>66</v>
       </c>
@@ -3126,32 +3126,32 @@
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="44"/>
+      <c r="H29" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N29" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="31"/>
-      <c r="H29" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="O29" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="P29" s="29"/>
+      <c r="O29" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="P29" s="36"/>
       <c r="Q29" s="6" t="s">
         <v>66</v>
       </c>
@@ -3174,17 +3174,17 @@
       <c r="R30" s="6"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C31" s="34" t="s">
-        <v>90</v>
+      <c r="C31" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H31" s="20" t="s">
         <v>67</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>66</v>
@@ -3198,9 +3198,9 @@
       <c r="R31" s="6"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C32" s="35"/>
+      <c r="C32" s="33"/>
       <c r="D32" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
@@ -3229,6 +3229,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O21:P21"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="L2:R2"/>
@@ -3245,13 +3252,6 @@
     <mergeCell ref="O17:P17"/>
     <mergeCell ref="O19:P19"/>
     <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O21:P21"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3262,403 +3262,403 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
+      <c r="D3" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="E3" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="H3" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45" t="s">
+      <c r="I3" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="C4" s="30">
+        <v>1</v>
+      </c>
+      <c r="D4" s="30">
+        <v>9</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30">
+        <v>12</v>
+      </c>
+      <c r="H4" s="30">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
+        <v>0</v>
+      </c>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="45" t="s">
+      <c r="C5" s="30">
+        <v>1</v>
+      </c>
+      <c r="D5" s="30">
+        <v>12</v>
+      </c>
+      <c r="E5" s="30">
+        <v>0.12</v>
+      </c>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30">
+        <v>12</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0.12</v>
+      </c>
+      <c r="I5" s="30">
+        <v>0.12</v>
+      </c>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C6" s="30">
         <v>1</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30">
+        <v>12</v>
+      </c>
+      <c r="H6" s="30">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30">
+        <v>0</v>
+      </c>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="30">
+        <v>1</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30">
+        <v>12</v>
+      </c>
+      <c r="H7" s="30">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30">
+        <v>0</v>
+      </c>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="30">
+        <v>1</v>
+      </c>
+      <c r="D8" s="30">
+        <v>5</v>
+      </c>
+      <c r="E8" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30">
+        <v>12</v>
+      </c>
+      <c r="H8" s="30">
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="I8" s="30">
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="30">
+        <v>1</v>
+      </c>
+      <c r="D9" s="30">
         <v>9</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45">
+      <c r="E9" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30">
         <v>12</v>
       </c>
-      <c r="H4" s="45">
-        <v>0</v>
-      </c>
-      <c r="I4" s="45">
-        <v>0</v>
-      </c>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="45">
+      <c r="H9" s="30">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="I9" s="30">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="30">
+        <v>4</v>
+      </c>
+      <c r="D10" s="30">
+        <v>12</v>
+      </c>
+      <c r="E10" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30">
+        <v>12</v>
+      </c>
+      <c r="H10" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="I10" s="30">
+        <v>1.2</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="30">
         <v>1</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D11" s="30">
         <v>12</v>
       </c>
-      <c r="E5" s="45">
-        <v>0.12</v>
-      </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45">
+      <c r="E11" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30">
         <v>12</v>
       </c>
-      <c r="H5" s="45">
-        <v>0.12</v>
-      </c>
-      <c r="I5" s="45">
-        <v>0.12</v>
-      </c>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="45">
+      <c r="H11" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="I11" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="30">
         <v>1</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45">
+      <c r="D12" s="30">
         <v>12</v>
       </c>
-      <c r="H6" s="45">
-        <v>0</v>
-      </c>
-      <c r="I6" s="45">
-        <v>0</v>
-      </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="45">
-        <v>1</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45">
+      <c r="E12" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30">
         <v>12</v>
       </c>
-      <c r="H7" s="45">
-        <v>0</v>
-      </c>
-      <c r="I7" s="45">
-        <v>0</v>
-      </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="45">
-        <v>1</v>
-      </c>
-      <c r="D8" s="45">
-        <v>5</v>
-      </c>
-      <c r="E8" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45">
-        <v>12</v>
-      </c>
-      <c r="H8" s="45">
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="I8" s="45">
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="45">
-        <v>1</v>
-      </c>
-      <c r="D9" s="45">
-        <v>9</v>
-      </c>
-      <c r="E9" s="45">
-        <v>0.6</v>
-      </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45">
-        <v>12</v>
-      </c>
-      <c r="H9" s="45">
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="I9" s="45">
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="45">
+      <c r="H12" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="I12" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="30">
         <v>4</v>
       </c>
-      <c r="D10" s="45">
-        <v>12</v>
-      </c>
-      <c r="E10" s="45">
-        <v>0.3</v>
-      </c>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45">
-        <v>12</v>
-      </c>
-      <c r="H10" s="45">
-        <v>0.3</v>
-      </c>
-      <c r="I10" s="45">
-        <v>1.2</v>
-      </c>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="45">
-        <v>1</v>
-      </c>
-      <c r="D11" s="45">
-        <v>12</v>
-      </c>
-      <c r="E11" s="45">
-        <v>1.5</v>
-      </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45">
-        <v>12</v>
-      </c>
-      <c r="H11" s="45">
-        <v>1.5</v>
-      </c>
-      <c r="I11" s="45">
-        <v>1.5</v>
-      </c>
-      <c r="J11" s="45"/>
-      <c r="K11" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="45" t="s">
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="45">
-        <v>1</v>
-      </c>
-      <c r="D12" s="45">
-        <v>12</v>
-      </c>
-      <c r="E12" s="45">
-        <v>1.5</v>
-      </c>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45">
-        <v>12</v>
-      </c>
-      <c r="H12" s="45">
-        <v>1.5</v>
-      </c>
-      <c r="I12" s="45">
-        <v>1.5</v>
-      </c>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="45" t="s">
+      <c r="I14" s="30">
+        <v>5.8116666666666665</v>
+      </c>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="45">
-        <v>4</v>
-      </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45" t="s">
+      <c r="C15" s="30">
+        <v>5.5</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="I14" s="45">
-        <v>5.8116666666666665</v>
-      </c>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="45" t="s">
+      <c r="C16" s="30">
+        <v>22</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30">
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="45">
-        <v>5.5</v>
-      </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="45" t="s">
+      <c r="C18" s="31">
+        <v>3.7854889589905363</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="45">
-        <v>22</v>
-      </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45">
-        <v>3.3333333333333335</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="46">
-        <v>3.7854889589905363</v>
-      </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="45">
+      <c r="C19" s="30">
         <v>1362.7760252365931</v>
       </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>